<commit_message>
Changed R15 to 470 Ohm
</commit_message>
<xml_diff>
--- a/Parts/BOM_Arduino_Spot_Welder_V2.2.xlsx
+++ b/Parts/BOM_Arduino_Spot_Welder_V2.2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
   <si>
     <t>Quantity</t>
   </si>
@@ -290,6 +290,63 @@
   </si>
   <si>
     <t>from malectrics.eu</t>
+  </si>
+  <si>
+    <t>PCB Onprint</t>
+  </si>
+  <si>
+    <t>IRFB_7437</t>
+  </si>
+  <si>
+    <t>P1 MCP1407</t>
+  </si>
+  <si>
+    <t>Pulse_ADJ</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>P2, P3, Auto_Pulse, Mosfet_ CTRL1</t>
+  </si>
+  <si>
+    <t>Foot_Switch</t>
+  </si>
+  <si>
+    <t>Auto_Pulse</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Zener D3</t>
+  </si>
+  <si>
+    <t>R10, R11</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R1, R12</t>
+  </si>
+  <si>
+    <t>R2, R3, R4, R5, R6, R7, R8, R9</t>
+  </si>
+  <si>
+    <t>LED D2</t>
+  </si>
+  <si>
+    <t>Mosfet_CTRL, P4, P5, Arduino Nano</t>
   </si>
 </sst>
 </file>
@@ -371,7 +428,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -420,7 +477,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FFCCCCCC"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
@@ -438,7 +495,7 @@
         <color rgb="FFCCCCCC"/>
       </left>
       <right style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
@@ -450,15 +507,26 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -470,6 +538,176 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -477,14 +715,66 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -493,159 +783,13 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -653,7 +797,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -695,91 +839,88 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -799,6 +940,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1104,620 +1281,691 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H40"/>
+  <dimension ref="B2:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="85.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="85.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E2" s="3" t="s">
+    <row r="2" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="16" t="s">
+    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="I4" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="19">
+    <row r="5" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="18">
         <v>8</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="15">
+      <c r="G5" s="15">
         <v>1.2</v>
       </c>
-      <c r="G5" s="15">
+      <c r="H5" s="15">
         <v>9.6</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="I5" s="19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="21">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="20">
+        <v>1</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10">
         <v>0.99</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="I6" s="21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-      <c r="C7" s="21">
-        <v>1</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="20">
+        <v>1</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10">
         <v>0.76</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="I7" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="21">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9" t="s">
+    <row r="8" spans="2:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="20">
+        <v>1</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10">
+      <c r="G8" s="9"/>
+      <c r="H8" s="10">
         <v>0.9</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="I8" s="21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="21">
+    <row r="9" spans="2:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="20">
         <v>3</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="10">
+      <c r="G9" s="10">
         <v>0.27</v>
       </c>
-      <c r="G9" s="10">
+      <c r="H9" s="10">
         <v>0.81</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="I9" s="21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="21">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9" t="s">
+    <row r="10" spans="2:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="20">
+        <v>1</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10">
+      <c r="G10" s="9"/>
+      <c r="H10" s="10">
         <v>0.17</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="I10" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="21">
-        <v>1</v>
-      </c>
-      <c r="D11" s="9" t="s">
+    <row r="11" spans="2:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="20">
+        <v>1</v>
+      </c>
+      <c r="D11" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="10">
+      <c r="G11" s="9"/>
+      <c r="H11" s="10">
         <v>0.26</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="I11" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="21">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9" t="s">
+    <row r="12" spans="2:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="20">
+        <v>1</v>
+      </c>
+      <c r="D12" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10">
+      <c r="G12" s="9"/>
+      <c r="H12" s="10">
         <v>0.02</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="I12" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="21">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9" t="s">
+    <row r="13" spans="2:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="20">
+        <v>1</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10">
+      <c r="G13" s="10"/>
+      <c r="H13" s="10">
         <v>0.04</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="I13" s="21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="21">
-        <v>1</v>
-      </c>
-      <c r="D14" s="50" t="s">
+    <row r="14" spans="2:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="20">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10">
+      <c r="G14" s="9"/>
+      <c r="H14" s="10">
         <v>0.08</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="I14" s="21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="21">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9" t="s">
+    <row r="15" spans="2:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="20">
+        <v>1</v>
+      </c>
+      <c r="D15" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="F15" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="10">
+      <c r="G15" s="9"/>
+      <c r="H15" s="10">
         <v>0.32</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="I15" s="21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="21">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9" t="s">
+    <row r="16" spans="2:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="20">
+        <v>1</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10">
+      <c r="G16" s="9"/>
+      <c r="H16" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="I16" s="21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="21">
-        <v>1</v>
-      </c>
-      <c r="D17" s="50" t="s">
+    <row r="17" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="20">
+        <v>1</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="F17" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10">
+      <c r="G17" s="10"/>
+      <c r="H17" s="10">
         <v>0.04</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="I17" s="21" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="21">
+    <row r="18" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="20">
         <v>2</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="58" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="F18" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="10">
+      <c r="G18" s="10">
         <v>0.02</v>
       </c>
-      <c r="G18" s="10">
+      <c r="H18" s="10">
         <v>0.04</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="I18" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="21">
-        <v>1</v>
-      </c>
-      <c r="D19" s="9" t="s">
+    <row r="19" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="20">
+        <v>1</v>
+      </c>
+      <c r="D19" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="F19" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10">
+      <c r="G19" s="10"/>
+      <c r="H19" s="10">
         <v>0.03</v>
       </c>
-      <c r="H19" s="22" t="s">
+      <c r="I19" s="21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="21">
-        <v>1</v>
-      </c>
-      <c r="D20" s="9" t="s">
+    <row r="20" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10">
+      <c r="G20" s="10"/>
+      <c r="H20" s="10">
         <v>0.02</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="I20" s="21" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="21">
+    <row r="21" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="20">
         <v>2</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="9">
+      <c r="G21" s="9">
         <v>0.02</v>
       </c>
-      <c r="G21" s="10">
+      <c r="H21" s="10">
         <v>0.04</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="I21" s="22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="21">
+    <row r="22" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="20">
         <v>8</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="67" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="9">
+      <c r="G22" s="9">
         <v>0.02</v>
       </c>
-      <c r="G22" s="10">
+      <c r="H22" s="10">
         <v>0.16</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="I22" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="3:8" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="24">
-        <v>1</v>
-      </c>
-      <c r="D23" s="25" t="s">
+    <row r="23" spans="3:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="F23" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28">
+      <c r="G23" s="26"/>
+      <c r="H23" s="27">
         <v>0.08</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="I23" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="53" t="s">
+    <row r="24" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G24" s="54">
-        <f>SUM(G5:G23)</f>
+      <c r="H24" s="53">
+        <f>SUM(H5:H23)</f>
         <v>14.429999999999996</v>
       </c>
     </row>
-    <row r="25" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="52"/>
-      <c r="G25" s="51"/>
-    </row>
-    <row r="26" spans="3:8" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="51"/>
+      <c r="H25" s="50"/>
+    </row>
+    <row r="26" spans="3:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="3:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="30">
-        <v>1</v>
-      </c>
-      <c r="D27" s="31" t="s">
+    <row r="27" spans="3:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="29">
+        <v>1</v>
+      </c>
+      <c r="D27" s="61"/>
+      <c r="E27" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33">
+      <c r="F27" s="30"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="32">
         <v>2</v>
       </c>
-      <c r="H27" s="34" t="s">
+      <c r="I27" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="21">
-        <v>1</v>
-      </c>
-      <c r="D28" s="9" t="s">
+    <row r="28" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="20">
+        <v>1</v>
+      </c>
+      <c r="D28" s="58"/>
+      <c r="E28" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="F28" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="11">
+      <c r="G28" s="9"/>
+      <c r="H28" s="11">
         <v>2</v>
       </c>
-      <c r="H28" s="36" t="s">
+      <c r="I28" s="35" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="21">
-        <v>1</v>
-      </c>
-      <c r="D29" s="9" t="s">
+    <row r="29" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="20">
+        <v>1</v>
+      </c>
+      <c r="D29" s="58"/>
+      <c r="E29" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="9"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="11">
+      <c r="G29" s="9"/>
+      <c r="H29" s="11">
         <v>3</v>
       </c>
-      <c r="H29" s="36" t="s">
+      <c r="I29" s="35" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="21">
-        <v>1</v>
-      </c>
-      <c r="D30" s="9" t="s">
+    <row r="30" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="20">
+        <v>1</v>
+      </c>
+      <c r="D30" s="58"/>
+      <c r="E30" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="F30" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="11">
-        <v>1</v>
-      </c>
-      <c r="H30" s="35" t="s">
+      <c r="G30" s="9"/>
+      <c r="H30" s="11">
+        <v>1</v>
+      </c>
+      <c r="I30" s="34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="21">
+    <row r="31" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="20">
         <v>3</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="58"/>
+      <c r="E31" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9">
+      <c r="F31" s="9"/>
+      <c r="G31" s="9">
         <v>0.6</v>
       </c>
-      <c r="G31" s="10">
+      <c r="H31" s="10">
         <v>1.8</v>
       </c>
-      <c r="H31" s="36" t="s">
+      <c r="I31" s="35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="37">
-        <v>1</v>
-      </c>
-      <c r="D32" s="6" t="s">
+    <row r="32" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="36">
+        <v>1</v>
+      </c>
+      <c r="D32" s="62"/>
+      <c r="E32" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8">
+      <c r="G32" s="7"/>
+      <c r="H32" s="8">
         <v>1.95</v>
       </c>
-      <c r="H32" s="38" t="s">
+      <c r="I32" s="37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="42">
-        <v>1</v>
-      </c>
-      <c r="D33" s="43" t="s">
+    <row r="33" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="41">
+        <v>1</v>
+      </c>
+      <c r="D33" s="63"/>
+      <c r="E33" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="44" t="s">
+      <c r="F33" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="F33" s="44"/>
-      <c r="G33" s="45">
+      <c r="G33" s="43"/>
+      <c r="H33" s="44">
         <v>5.8</v>
       </c>
-      <c r="H33" s="49" t="s">
+      <c r="I33" s="48" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="37">
-        <v>1</v>
-      </c>
-      <c r="D34" s="9" t="s">
+    <row r="34" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="36">
+        <v>1</v>
+      </c>
+      <c r="D34" s="62"/>
+      <c r="E34" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8">
+      <c r="G34" s="7"/>
+      <c r="H34" s="8">
         <v>4.57</v>
       </c>
-      <c r="H34" s="46" t="s">
+      <c r="I34" s="45" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="3:8" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="39">
-        <v>1</v>
-      </c>
-      <c r="D35" s="25" t="s">
+    <row r="35" spans="3:9" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="38">
+        <v>1</v>
+      </c>
+      <c r="D35" s="64"/>
+      <c r="E35" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="40" t="s">
+      <c r="F35" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="27"/>
-      <c r="G35" s="41">
+      <c r="G35" s="26"/>
+      <c r="H35" s="40">
         <v>2.0099999999999998</v>
       </c>
-      <c r="H35" s="47" t="s">
+      <c r="I35" s="46" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="55" t="s">
+    <row r="36" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="G36" s="56">
-        <f>SUM(G27:G35)</f>
+      <c r="H36" s="55">
+        <f>SUM(H27:H35)</f>
         <v>24.130000000000003</v>
       </c>
     </row>
-    <row r="37" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E38" s="3" t="s">
+    <row r="37" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F38" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G38" s="56">
-        <f>SUM(G24,G36)</f>
+      <c r="H38" s="55">
+        <f>SUM(H24,H36)</f>
         <v>38.56</v>
       </c>
     </row>
-    <row r="39" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="3:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="3:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H7" r:id="rId1"/>
-    <hyperlink ref="H8" r:id="rId2"/>
-    <hyperlink ref="H9" r:id="rId3"/>
-    <hyperlink ref="H10" r:id="rId4"/>
-    <hyperlink ref="H13" r:id="rId5"/>
-    <hyperlink ref="H11" r:id="rId6"/>
-    <hyperlink ref="H2" r:id="rId7"/>
-    <hyperlink ref="H6" r:id="rId8"/>
-    <hyperlink ref="H21" r:id="rId9"/>
-    <hyperlink ref="H34" r:id="rId10"/>
-    <hyperlink ref="H35" r:id="rId11"/>
-    <hyperlink ref="E28" r:id="rId12"/>
-    <hyperlink ref="H15" r:id="rId13"/>
-    <hyperlink ref="H5" r:id="rId14"/>
+    <hyperlink ref="I7" r:id="rId1"/>
+    <hyperlink ref="I8" r:id="rId2"/>
+    <hyperlink ref="I9" r:id="rId3"/>
+    <hyperlink ref="I10" r:id="rId4"/>
+    <hyperlink ref="I13" r:id="rId5"/>
+    <hyperlink ref="I11" r:id="rId6"/>
+    <hyperlink ref="I2" r:id="rId7"/>
+    <hyperlink ref="I6" r:id="rId8"/>
+    <hyperlink ref="I21" r:id="rId9"/>
+    <hyperlink ref="I34" r:id="rId10"/>
+    <hyperlink ref="I35" r:id="rId11"/>
+    <hyperlink ref="F28" r:id="rId12"/>
+    <hyperlink ref="I15" r:id="rId13"/>
+    <hyperlink ref="I5" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>

</xml_diff>